<commit_message>
09-0480 taken off remove
</commit_message>
<xml_diff>
--- a/dependencies/mycobacterium/tbc/af2122/script_dependents/RemoveFromAnalysis.xlsx
+++ b/dependencies/mycobacterium/tbc/af2122/script_dependents/RemoveFromAnalysis.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11015"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Q:\TStuber\Results\mycobacterium\tbc\af2122\script_dependents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tstuber/workspace/vSNP/dependencies/mycobacterium/tbc/af2122/script_dependents/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8CA6B79-ECBC-EB45-813F-52BD09DF261F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="68355" yWindow="9225" windowWidth="21045" windowHeight="14745" tabRatio="500"/>
+    <workbookView xWindow="7760" yWindow="2460" windowWidth="21040" windowHeight="14740" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="250">
   <si>
     <t>13-8081</t>
   </si>
@@ -771,12 +772,15 @@
   </si>
   <si>
     <t>duplicate of 16-014019-008-B3_UG; 16-014019-011-B4_UG</t>
+  </si>
+  <si>
+    <t>moved out 2018-10-20, a question to if it is the same isolate as 09-0480 and is related to 07-6182</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1097,276 +1101,276 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B200"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E200"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A132" workbookViewId="0">
-      <selection activeCell="A180" sqref="A180"/>
+    <sheetView tabSelected="1" topLeftCell="B136" workbookViewId="0">
+      <selection activeCell="G158" sqref="G158"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="46.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="83.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="10.875" style="1"/>
+    <col min="1" max="1" width="46.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="83.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>74</v>
       </c>
@@ -1374,7 +1378,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>76</v>
       </c>
@@ -1382,62 +1386,62 @@
         <v>75</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>77</v>
       </c>
@@ -1445,7 +1449,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>79</v>
       </c>
@@ -1453,7 +1457,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>81</v>
       </c>
@@ -1461,7 +1465,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>82</v>
       </c>
@@ -1469,7 +1473,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>161</v>
       </c>
@@ -1477,7 +1481,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>84</v>
       </c>
@@ -1485,7 +1489,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>85</v>
       </c>
@@ -1493,7 +1497,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>162</v>
       </c>
@@ -1501,7 +1505,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>163</v>
       </c>
@@ -1509,7 +1513,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>88</v>
       </c>
@@ -1517,7 +1521,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>90</v>
       </c>
@@ -1525,7 +1529,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>92</v>
       </c>
@@ -1533,7 +1537,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>94</v>
       </c>
@@ -1541,7 +1545,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>96</v>
       </c>
@@ -1549,7 +1553,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>98</v>
       </c>
@@ -1557,7 +1561,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>100</v>
       </c>
@@ -1565,7 +1569,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>102</v>
       </c>
@@ -1573,7 +1577,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>104</v>
       </c>
@@ -1581,7 +1585,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
         <v>106</v>
       </c>
@@ -1589,7 +1593,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
         <v>107</v>
       </c>
@@ -1597,7 +1601,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
         <v>108</v>
       </c>
@@ -1605,7 +1609,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>110</v>
       </c>
@@ -1613,7 +1617,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
         <v>111</v>
       </c>
@@ -1621,7 +1625,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
         <v>112</v>
       </c>
@@ -1629,7 +1633,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
         <v>114</v>
       </c>
@@ -1637,7 +1641,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
         <v>115</v>
       </c>
@@ -1645,7 +1649,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
         <v>116</v>
       </c>
@@ -1653,7 +1657,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
         <v>117</v>
       </c>
@@ -1661,7 +1665,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
         <v>118</v>
       </c>
@@ -1669,7 +1673,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
         <v>119</v>
       </c>
@@ -1677,7 +1681,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
         <v>120</v>
       </c>
@@ -1685,7 +1689,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
         <v>121</v>
       </c>
@@ -1693,7 +1697,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
         <v>122</v>
       </c>
@@ -1701,7 +1705,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
         <v>123</v>
       </c>
@@ -1709,7 +1713,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
         <v>124</v>
       </c>
@@ -1717,7 +1721,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
         <v>125</v>
       </c>
@@ -1725,7 +1729,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
         <v>126</v>
       </c>
@@ -1733,7 +1737,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
         <v>127</v>
       </c>
@@ -1741,7 +1745,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
         <v>128</v>
       </c>
@@ -1749,7 +1753,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
         <v>129</v>
       </c>
@@ -1757,7 +1761,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
         <v>130</v>
       </c>
@@ -1765,7 +1769,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
         <v>131</v>
       </c>
@@ -1773,7 +1777,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
         <v>133</v>
       </c>
@@ -1781,7 +1785,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
         <v>135</v>
       </c>
@@ -1789,7 +1793,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
         <v>137</v>
       </c>
@@ -1797,7 +1801,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
         <v>139</v>
       </c>
@@ -1805,7 +1809,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
         <v>164</v>
       </c>
@@ -1813,7 +1817,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
         <v>142</v>
       </c>
@@ -1821,7 +1825,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
         <v>144</v>
       </c>
@@ -1829,7 +1833,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
         <v>146</v>
       </c>
@@ -1837,7 +1841,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
         <v>148</v>
       </c>
@@ -1845,7 +1849,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
         <v>149</v>
       </c>
@@ -1853,7 +1857,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
         <v>165</v>
       </c>
@@ -1861,7 +1865,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
         <v>166</v>
       </c>
@@ -1869,7 +1873,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
         <v>152</v>
       </c>
@@ -1877,7 +1881,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
         <v>172</v>
       </c>
@@ -1885,7 +1889,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
         <v>174</v>
       </c>
@@ -1893,7 +1897,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
         <v>167</v>
       </c>
@@ -1901,7 +1905,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
         <v>168</v>
       </c>
@@ -1909,7 +1913,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
         <v>169</v>
       </c>
@@ -1917,7 +1921,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
         <v>170</v>
       </c>
@@ -1925,7 +1929,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
         <v>155</v>
       </c>
@@ -1933,7 +1937,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
         <v>156</v>
       </c>
@@ -1941,7 +1945,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
         <v>157</v>
       </c>
@@ -1949,7 +1953,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
         <v>158</v>
       </c>
@@ -1957,7 +1961,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
         <v>159</v>
       </c>
@@ -1965,7 +1969,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
         <v>160</v>
       </c>
@@ -1973,7 +1977,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="s">
         <v>71</v>
       </c>
@@ -1981,7 +1985,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
         <v>59</v>
       </c>
@@ -1989,7 +1993,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
         <v>72</v>
       </c>
@@ -1997,7 +2001,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A135" s="1" t="s">
         <v>73</v>
       </c>
@@ -2005,7 +2009,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="s">
         <v>60</v>
       </c>
@@ -2013,7 +2017,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A137" s="1" t="s">
         <v>61</v>
       </c>
@@ -2021,7 +2025,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A138" s="1" t="s">
         <v>62</v>
       </c>
@@ -2029,7 +2033,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A139" s="1" t="s">
         <v>63</v>
       </c>
@@ -2037,7 +2041,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A140" s="1" t="s">
         <v>64</v>
       </c>
@@ -2045,7 +2049,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A141" s="1" t="s">
         <v>65</v>
       </c>
@@ -2053,7 +2057,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A142" s="1" t="s">
         <v>66</v>
       </c>
@@ -2061,7 +2065,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A143" s="1" t="s">
         <v>176</v>
       </c>
@@ -2069,7 +2073,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A144" s="1" t="s">
         <v>178</v>
       </c>
@@ -2077,7 +2081,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A145" s="1" t="s">
         <v>180</v>
       </c>
@@ -2085,7 +2089,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A146" s="1" t="s">
         <v>182</v>
       </c>
@@ -2093,7 +2097,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A147" s="1" t="s">
         <v>184</v>
       </c>
@@ -2101,7 +2105,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A148" s="1" t="s">
         <v>186</v>
       </c>
@@ -2109,12 +2113,12 @@
         <v>185</v>
       </c>
     </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A149" s="1" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>188</v>
       </c>
@@ -2122,7 +2126,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>189</v>
       </c>
@@ -2130,15 +2134,18 @@
         <v>190</v>
       </c>
     </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A152" s="1" t="s">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C152" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="B152" s="1" t="s">
+      <c r="D152" s="1" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E152" s="1" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A153" s="1" t="s">
         <v>193</v>
       </c>
@@ -2146,7 +2153,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A154" s="1" t="s">
         <v>194</v>
       </c>
@@ -2154,7 +2161,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A155" s="1" t="s">
         <v>195</v>
       </c>
@@ -2162,7 +2169,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A156" s="1" t="s">
         <v>196</v>
       </c>
@@ -2170,7 +2177,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A157" s="1" t="s">
         <v>197</v>
       </c>
@@ -2178,7 +2185,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A158" s="1" t="s">
         <v>198</v>
       </c>
@@ -2186,7 +2193,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A159" s="1" t="s">
         <v>199</v>
       </c>
@@ -2194,7 +2201,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="160" spans="1:2" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:5" ht="20" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
         <v>200</v>
       </c>
@@ -2202,7 +2209,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A161" s="1" t="s">
         <v>203</v>
       </c>
@@ -2210,7 +2217,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A162" s="1" t="s">
         <v>204</v>
       </c>
@@ -2218,7 +2225,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A163" s="1" t="s">
         <v>206</v>
       </c>
@@ -2226,7 +2233,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A164" s="1" t="s">
         <v>207</v>
       </c>
@@ -2234,7 +2241,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A165" s="1" t="s">
         <v>208</v>
       </c>
@@ -2242,7 +2249,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A166" s="1" t="s">
         <v>209</v>
       </c>
@@ -2250,7 +2257,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>210</v>
       </c>
@@ -2258,7 +2265,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>211</v>
       </c>
@@ -2266,7 +2273,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>212</v>
       </c>
@@ -2274,7 +2281,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>213</v>
       </c>
@@ -2282,7 +2289,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>214</v>
       </c>
@@ -2290,7 +2297,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>215</v>
       </c>
@@ -2298,7 +2305,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>216</v>
       </c>
@@ -2306,7 +2313,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>217</v>
       </c>
@@ -2314,7 +2321,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>218</v>
       </c>
@@ -2322,7 +2329,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A176" s="1" t="s">
         <v>219</v>
       </c>
@@ -2330,7 +2337,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A177" s="1" t="s">
         <v>220</v>
       </c>
@@ -2338,7 +2345,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A178" s="1" t="s">
         <v>221</v>
       </c>
@@ -2346,7 +2353,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A179" s="1" t="s">
         <v>222</v>
       </c>
@@ -2354,7 +2361,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A180" s="1" t="s">
         <v>223</v>
       </c>
@@ -2362,7 +2369,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A181" s="1" t="s">
         <v>224</v>
       </c>
@@ -2370,7 +2377,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A182" s="1" t="s">
         <v>226</v>
       </c>
@@ -2378,7 +2385,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A183" s="1" t="s">
         <v>227</v>
       </c>
@@ -2386,7 +2393,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A184" s="1" t="s">
         <v>228</v>
       </c>
@@ -2394,7 +2401,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>229</v>
       </c>
@@ -2402,7 +2409,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>230</v>
       </c>
@@ -2410,7 +2417,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>231</v>
       </c>
@@ -2418,7 +2425,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>232</v>
       </c>
@@ -2426,7 +2433,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>233</v>
       </c>
@@ -2434,7 +2441,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>234</v>
       </c>
@@ -2442,7 +2449,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>235</v>
       </c>
@@ -2450,7 +2457,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>236</v>
       </c>
@@ -2458,7 +2465,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>237</v>
       </c>
@@ -2466,7 +2473,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>238</v>
       </c>
@@ -2474,7 +2481,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>239</v>
       </c>
@@ -2482,7 +2489,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A196" s="1" t="s">
         <v>241</v>
       </c>
@@ -2490,7 +2497,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A197" s="1" t="s">
         <v>242</v>
       </c>
@@ -2498,7 +2505,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>243</v>
       </c>
@@ -2506,7 +2513,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A199" s="1" t="s">
         <v>245</v>
       </c>
@@ -2514,7 +2521,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A200" s="1" t="s">
         <v>247</v>
       </c>

</xml_diff>

<commit_message>
fix for virus filter and remove_from
</commit_message>
<xml_diff>
--- a/dependencies/mycobacterium/tbc/af2122/script_dependents/RemoveFromAnalysis.xlsx
+++ b/dependencies/mycobacterium/tbc/af2122/script_dependents/RemoveFromAnalysis.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11015"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Q:\TStuber\Results\mycobacterium\tbc\af2122\script_dependents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tstuber/workspace/vSNP/dependencies/mycobacterium/tbc/af2122/script_dependents/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45BAE34E-6232-9348-8663-FB3FF4BA6F97}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="68355" yWindow="9225" windowWidth="21045" windowHeight="14745" tabRatio="500"/>
+    <workbookView xWindow="7760" yWindow="2460" windowWidth="21040" windowHeight="14740" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="250">
   <si>
     <t>13-8081</t>
   </si>
@@ -771,12 +772,15 @@
   </si>
   <si>
     <t>duplicate of 16-014019-008-B3_UG; 16-014019-011-B4_UG</t>
+  </si>
+  <si>
+    <t>isolate back into analysis 2018-10-20.  Confusion as if the isolate is same as 09-0480.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1097,276 +1101,276 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B200"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E200"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A132" workbookViewId="0">
-      <selection activeCell="A180" sqref="A180"/>
+    <sheetView tabSelected="1" topLeftCell="B136" workbookViewId="0">
+      <selection activeCell="B152" sqref="B152"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="46.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="83.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="10.875" style="1"/>
+    <col min="1" max="1" width="46.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="83.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>74</v>
       </c>
@@ -1374,7 +1378,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>76</v>
       </c>
@@ -1382,62 +1386,62 @@
         <v>75</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>77</v>
       </c>
@@ -1445,7 +1449,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>79</v>
       </c>
@@ -1453,7 +1457,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>81</v>
       </c>
@@ -1461,7 +1465,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>82</v>
       </c>
@@ -1469,7 +1473,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>161</v>
       </c>
@@ -1477,7 +1481,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>84</v>
       </c>
@@ -1485,7 +1489,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>85</v>
       </c>
@@ -1493,7 +1497,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>162</v>
       </c>
@@ -1501,7 +1505,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>163</v>
       </c>
@@ -1509,7 +1513,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>88</v>
       </c>
@@ -1517,7 +1521,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>90</v>
       </c>
@@ -1525,7 +1529,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>92</v>
       </c>
@@ -1533,7 +1537,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>94</v>
       </c>
@@ -1541,7 +1545,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>96</v>
       </c>
@@ -1549,7 +1553,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>98</v>
       </c>
@@ -1557,7 +1561,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>100</v>
       </c>
@@ -1565,7 +1569,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>102</v>
       </c>
@@ -1573,7 +1577,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>104</v>
       </c>
@@ -1581,7 +1585,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
         <v>106</v>
       </c>
@@ -1589,7 +1593,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
         <v>107</v>
       </c>
@@ -1597,7 +1601,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
         <v>108</v>
       </c>
@@ -1605,7 +1609,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>110</v>
       </c>
@@ -1613,7 +1617,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
         <v>111</v>
       </c>
@@ -1621,7 +1625,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
         <v>112</v>
       </c>
@@ -1629,7 +1633,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
         <v>114</v>
       </c>
@@ -1637,7 +1641,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
         <v>115</v>
       </c>
@@ -1645,7 +1649,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
         <v>116</v>
       </c>
@@ -1653,7 +1657,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
         <v>117</v>
       </c>
@@ -1661,7 +1665,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
         <v>118</v>
       </c>
@@ -1669,7 +1673,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
         <v>119</v>
       </c>
@@ -1677,7 +1681,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
         <v>120</v>
       </c>
@@ -1685,7 +1689,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
         <v>121</v>
       </c>
@@ -1693,7 +1697,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
         <v>122</v>
       </c>
@@ -1701,7 +1705,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
         <v>123</v>
       </c>
@@ -1709,7 +1713,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
         <v>124</v>
       </c>
@@ -1717,7 +1721,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
         <v>125</v>
       </c>
@@ -1725,7 +1729,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
         <v>126</v>
       </c>
@@ -1733,7 +1737,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
         <v>127</v>
       </c>
@@ -1741,7 +1745,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
         <v>128</v>
       </c>
@@ -1749,7 +1753,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
         <v>129</v>
       </c>
@@ -1757,7 +1761,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
         <v>130</v>
       </c>
@@ -1765,7 +1769,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
         <v>131</v>
       </c>
@@ -1773,7 +1777,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
         <v>133</v>
       </c>
@@ -1781,7 +1785,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
         <v>135</v>
       </c>
@@ -1789,7 +1793,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
         <v>137</v>
       </c>
@@ -1797,7 +1801,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
         <v>139</v>
       </c>
@@ -1805,7 +1809,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
         <v>164</v>
       </c>
@@ -1813,7 +1817,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
         <v>142</v>
       </c>
@@ -1821,7 +1825,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
         <v>144</v>
       </c>
@@ -1829,7 +1833,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
         <v>146</v>
       </c>
@@ -1837,7 +1841,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
         <v>148</v>
       </c>
@@ -1845,7 +1849,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
         <v>149</v>
       </c>
@@ -1853,7 +1857,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
         <v>165</v>
       </c>
@@ -1861,7 +1865,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
         <v>166</v>
       </c>
@@ -1869,7 +1873,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
         <v>152</v>
       </c>
@@ -1877,7 +1881,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
         <v>172</v>
       </c>
@@ -1885,7 +1889,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
         <v>174</v>
       </c>
@@ -1893,7 +1897,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
         <v>167</v>
       </c>
@@ -1901,7 +1905,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
         <v>168</v>
       </c>
@@ -1909,7 +1913,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
         <v>169</v>
       </c>
@@ -1917,7 +1921,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
         <v>170</v>
       </c>
@@ -1925,7 +1929,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
         <v>155</v>
       </c>
@@ -1933,7 +1937,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
         <v>156</v>
       </c>
@@ -1941,7 +1945,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
         <v>157</v>
       </c>
@@ -1949,7 +1953,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
         <v>158</v>
       </c>
@@ -1957,7 +1961,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
         <v>159</v>
       </c>
@@ -1965,7 +1969,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
         <v>160</v>
       </c>
@@ -1973,7 +1977,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="s">
         <v>71</v>
       </c>
@@ -1981,7 +1985,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
         <v>59</v>
       </c>
@@ -1989,7 +1993,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
         <v>72</v>
       </c>
@@ -1997,7 +2001,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A135" s="1" t="s">
         <v>73</v>
       </c>
@@ -2005,7 +2009,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="s">
         <v>60</v>
       </c>
@@ -2013,7 +2017,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A137" s="1" t="s">
         <v>61</v>
       </c>
@@ -2021,7 +2025,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A138" s="1" t="s">
         <v>62</v>
       </c>
@@ -2029,7 +2033,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A139" s="1" t="s">
         <v>63</v>
       </c>
@@ -2037,7 +2041,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A140" s="1" t="s">
         <v>64</v>
       </c>
@@ -2045,7 +2049,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A141" s="1" t="s">
         <v>65</v>
       </c>
@@ -2053,7 +2057,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A142" s="1" t="s">
         <v>66</v>
       </c>
@@ -2061,7 +2065,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A143" s="1" t="s">
         <v>176</v>
       </c>
@@ -2069,7 +2073,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A144" s="1" t="s">
         <v>178</v>
       </c>
@@ -2077,7 +2081,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A145" s="1" t="s">
         <v>180</v>
       </c>
@@ -2085,7 +2089,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A146" s="1" t="s">
         <v>182</v>
       </c>
@@ -2093,7 +2097,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A147" s="1" t="s">
         <v>184</v>
       </c>
@@ -2101,7 +2105,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A148" s="1" t="s">
         <v>186</v>
       </c>
@@ -2109,12 +2113,12 @@
         <v>185</v>
       </c>
     </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A149" s="1" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>188</v>
       </c>
@@ -2122,7 +2126,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>189</v>
       </c>
@@ -2130,15 +2134,18 @@
         <v>190</v>
       </c>
     </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A152" s="1" t="s">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C152" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="B152" s="1" t="s">
+      <c r="D152" s="1" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E152" s="1" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A153" s="1" t="s">
         <v>193</v>
       </c>
@@ -2146,7 +2153,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A154" s="1" t="s">
         <v>194</v>
       </c>
@@ -2154,7 +2161,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A155" s="1" t="s">
         <v>195</v>
       </c>
@@ -2162,7 +2169,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A156" s="1" t="s">
         <v>196</v>
       </c>
@@ -2170,7 +2177,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A157" s="1" t="s">
         <v>197</v>
       </c>
@@ -2178,7 +2185,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A158" s="1" t="s">
         <v>198</v>
       </c>
@@ -2186,7 +2193,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A159" s="1" t="s">
         <v>199</v>
       </c>
@@ -2194,7 +2201,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="160" spans="1:2" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:5" ht="20" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
         <v>200</v>
       </c>
@@ -2202,7 +2209,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A161" s="1" t="s">
         <v>203</v>
       </c>
@@ -2210,7 +2217,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A162" s="1" t="s">
         <v>204</v>
       </c>
@@ -2218,7 +2225,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A163" s="1" t="s">
         <v>206</v>
       </c>
@@ -2226,7 +2233,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A164" s="1" t="s">
         <v>207</v>
       </c>
@@ -2234,7 +2241,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A165" s="1" t="s">
         <v>208</v>
       </c>
@@ -2242,7 +2249,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A166" s="1" t="s">
         <v>209</v>
       </c>
@@ -2250,7 +2257,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>210</v>
       </c>
@@ -2258,7 +2265,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>211</v>
       </c>
@@ -2266,7 +2273,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>212</v>
       </c>
@@ -2274,7 +2281,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>213</v>
       </c>
@@ -2282,7 +2289,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>214</v>
       </c>
@@ -2290,7 +2297,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>215</v>
       </c>
@@ -2298,7 +2305,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>216</v>
       </c>
@@ -2306,7 +2313,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>217</v>
       </c>
@@ -2314,7 +2321,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>218</v>
       </c>
@@ -2322,7 +2329,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A176" s="1" t="s">
         <v>219</v>
       </c>
@@ -2330,7 +2337,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A177" s="1" t="s">
         <v>220</v>
       </c>
@@ -2338,7 +2345,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A178" s="1" t="s">
         <v>221</v>
       </c>
@@ -2346,7 +2353,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A179" s="1" t="s">
         <v>222</v>
       </c>
@@ -2354,7 +2361,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A180" s="1" t="s">
         <v>223</v>
       </c>
@@ -2362,7 +2369,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A181" s="1" t="s">
         <v>224</v>
       </c>
@@ -2370,7 +2377,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A182" s="1" t="s">
         <v>226</v>
       </c>
@@ -2378,7 +2385,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A183" s="1" t="s">
         <v>227</v>
       </c>
@@ -2386,7 +2393,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A184" s="1" t="s">
         <v>228</v>
       </c>
@@ -2394,7 +2401,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>229</v>
       </c>
@@ -2402,7 +2409,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>230</v>
       </c>
@@ -2410,7 +2417,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>231</v>
       </c>
@@ -2418,7 +2425,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>232</v>
       </c>
@@ -2426,7 +2433,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>233</v>
       </c>
@@ -2434,7 +2441,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>234</v>
       </c>
@@ -2442,7 +2449,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>235</v>
       </c>
@@ -2450,7 +2457,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>236</v>
       </c>
@@ -2458,7 +2465,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>237</v>
       </c>
@@ -2466,7 +2473,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>238</v>
       </c>
@@ -2474,7 +2481,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>239</v>
       </c>
@@ -2482,7 +2489,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A196" s="1" t="s">
         <v>241</v>
       </c>
@@ -2490,7 +2497,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A197" s="1" t="s">
         <v>242</v>
       </c>
@@ -2498,7 +2505,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>243</v>
       </c>
@@ -2506,7 +2513,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A199" s="1" t="s">
         <v>245</v>
       </c>
@@ -2514,7 +2521,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A200" s="1" t="s">
         <v>247</v>
       </c>

</xml_diff>